<commit_message>
new results; ToT Objects and Naive
</commit_message>
<xml_diff>
--- a/results/tot_normal/arc_1D/manual_task_analysis.xlsx
+++ b/results/tot_normal/arc_1D/manual_task_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Universität\Mannheim\Studium\5. Semester HWS\Masterthesis\results\tot_normal\arc_1D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9FF921-A57C-4D14-8552-DF7904491996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6B57F5-FB62-4053-9A98-E68F0A2C13DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0EC1F964-009C-44AA-8331-5AE0B72718BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="5" activeTab="6" xr2:uid="{0EC1F964-009C-44AA-8331-5AE0B72718BA}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="129">
   <si>
     <t>task_name</t>
   </si>
@@ -294,9 +294,6 @@
     <t>recolor_cmp</t>
   </si>
   <si>
-    <t>description not wrong but brings model on wrong track</t>
-  </si>
-  <si>
     <t>1d_pcopy_1c_35.json</t>
   </si>
   <si>
@@ -330,9 +327,6 @@
     <t>1d_move_3p_47.json</t>
   </si>
   <si>
-    <t>description to generic</t>
-  </si>
-  <si>
     <t>1d_recolor_cmp_37.json</t>
   </si>
   <si>
@@ -345,9 +339,6 @@
     <t>1d_pcopy_1c_0.json</t>
   </si>
   <si>
-    <t>too generic description</t>
-  </si>
-  <si>
     <t>1d_recolor_cmp_2.json</t>
   </si>
   <si>
@@ -420,9 +411,6 @@
     <t>1d_recolor_cmp_4.json</t>
   </si>
   <si>
-    <t>description too generic</t>
-  </si>
-  <si>
     <t>1d_move_3p_7.json</t>
   </si>
   <si>
@@ -433,6 +421,15 @@
   </si>
   <si>
     <t>1d_denoising_1c_20.json</t>
+  </si>
+  <si>
+    <t>mistake in object detection lead to too generic description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description not wrong but too generic </t>
+  </si>
+  <si>
+    <t>description not wrong but too generic ; pattern wrong but randomly fit to test case</t>
   </si>
 </sst>
 </file>
@@ -456,12 +453,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -476,9 +479,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,10 +887,10 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -1543,9 +1548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C160EF6F-0555-4875-ACB1-014D97C824DF}">
   <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA7" sqref="AA7"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,10 +1635,10 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -1837,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="AN2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -2103,7 +2108,7 @@
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
@@ -2112,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>80</v>
@@ -2121,7 +2126,7 @@
         <v>80</v>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -2147,8 +2152,8 @@
       <c r="O5" t="b">
         <v>1</v>
       </c>
-      <c r="P5" t="b">
-        <v>1</v>
+      <c r="P5" t="s">
+        <v>80</v>
       </c>
       <c r="Q5" t="b">
         <v>1</v>
@@ -2208,7 +2213,7 @@
         <v>1</v>
       </c>
       <c r="AI5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5" t="b">
         <v>0</v>
@@ -2231,28 +2236,25 @@
         <v>82</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
-      <c r="E6" t="str">
-        <f t="shared" si="9"/>
-        <v>None</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="10"/>
-        <v>None</v>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
       </c>
       <c r="G6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" ref="I6:I10" si="12">IF(H6=TRUE,"","None")</f>
-        <v>None</v>
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -2274,8 +2276,8 @@
       <c r="O6" t="b">
         <v>1</v>
       </c>
-      <c r="P6" t="b">
-        <v>1</v>
+      <c r="P6" t="s">
+        <v>80</v>
       </c>
       <c r="Q6" t="b">
         <v>1</v>
@@ -2337,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="AI6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6" t="b">
         <v>0</v>
@@ -2351,16 +2353,13 @@
       <c r="AM6" t="b">
         <v>0</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>84</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
@@ -2486,7 +2485,7 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
@@ -2495,16 +2494,16 @@
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>80</v>
       </c>
-      <c r="F8" t="b">
-        <v>1</v>
+      <c r="F8" t="s">
+        <v>80</v>
       </c>
       <c r="G8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
@@ -2532,8 +2531,8 @@
       <c r="O8" t="b">
         <v>1</v>
       </c>
-      <c r="P8" t="b">
-        <v>0</v>
+      <c r="P8" t="s">
+        <v>80</v>
       </c>
       <c r="Q8" t="b">
         <v>1</v>
@@ -2608,13 +2607,10 @@
       <c r="AM8" t="b">
         <v>0</v>
       </c>
-      <c r="AN8" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>82</v>
@@ -2743,10 +2739,10 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2769,7 +2765,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="I6:I10" si="12">IF(H10=TRUE,"","None")</f>
         <v>None</v>
       </c>
       <c r="J10" t="b">
@@ -2870,7 +2866,7 @@
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
@@ -3007,9 +3003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1645F0D-2C42-4FDA-9EAC-EE98B635BBCE}">
   <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL5" sqref="AL5"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3094,10 +3090,10 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -3177,7 +3173,7 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
@@ -3298,12 +3294,12 @@
         <v>0</v>
       </c>
       <c r="AN2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
         <v>82</v>
@@ -3426,12 +3422,12 @@
         <v>0</v>
       </c>
       <c r="AN3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
         <v>75</v>
@@ -3558,11 +3554,11 @@
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>119</v>
+      <c r="A5" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -3683,11 +3679,11 @@
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>120</v>
+      <c r="A6" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -3810,11 +3806,11 @@
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>104</v>
+      <c r="A7" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -3941,7 +3937,7 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
         <v>75</v>
@@ -4067,11 +4063,11 @@
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>122</v>
+      <c r="A9" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -4197,8 +4193,8 @@
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>123</v>
+      <c r="A10" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B10" t="s">
         <v>77</v>
@@ -4323,8 +4319,8 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>110</v>
+      <c r="A11" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="B11" t="s">
         <v>77</v>
@@ -4460,9 +4456,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687D7031-258F-4DE2-A9D8-7479C0C678CF}">
   <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="AL1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4547,10 +4543,10 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -4629,8 +4625,8 @@
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>94</v>
+      <c r="A2" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
@@ -4639,16 +4635,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -4676,8 +4672,8 @@
       <c r="O2" t="b">
         <v>1</v>
       </c>
-      <c r="P2" t="b">
-        <v>0</v>
+      <c r="P2" t="s">
+        <v>80</v>
       </c>
       <c r="Q2" t="b">
         <v>1</v>
@@ -4739,7 +4735,7 @@
         <v>1</v>
       </c>
       <c r="AI2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2" t="b">
         <v>0</v>
@@ -4754,21 +4750,21 @@
         <v>0</v>
       </c>
       <c r="AN2" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E11" si="0">IF(OR(C3=FALSE,D3=FALSE),"None","")</f>
@@ -4779,14 +4775,13 @@
         <v>None</v>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I11" si="2">IF(H3=TRUE,"","None")</f>
-        <v>None</v>
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -4795,11 +4790,11 @@
         <v>0</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L10" si="3">IF(OR(J3=FALSE,K3=FALSE),"None","")</f>
+        <f t="shared" ref="L3:L10" si="2">IF(OR(J3=FALSE,K3=FALSE),"None","")</f>
         <v>None</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M10" si="4">IF(OR(J3=FALSE,K3=FALSE),"None","")</f>
+        <f t="shared" ref="M3:M10" si="3">IF(OR(J3=FALSE,K3=FALSE),"None","")</f>
         <v>None</v>
       </c>
       <c r="N3" t="b">
@@ -4808,8 +4803,8 @@
       <c r="O3" t="b">
         <v>1</v>
       </c>
-      <c r="P3" t="b">
-        <v>0</v>
+      <c r="P3" t="s">
+        <v>80</v>
       </c>
       <c r="Q3" t="b">
         <v>1</v>
@@ -4821,11 +4816,11 @@
         <v>0</v>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:T10" si="5">IF(OR(R3=FALSE,S3=FALSE),"None","")</f>
+        <f t="shared" ref="T3:T10" si="4">IF(OR(R3=FALSE,S3=FALSE),"None","")</f>
         <v>None</v>
       </c>
       <c r="U3" t="str">
-        <f t="shared" ref="U3:U10" si="6">IF(OR(R3=FALSE,S3=FALSE),"None","")</f>
+        <f t="shared" ref="U3:U10" si="5">IF(OR(R3=FALSE,S3=FALSE),"None","")</f>
         <v>None</v>
       </c>
       <c r="V3" t="b">
@@ -4844,11 +4839,11 @@
         <v>0</v>
       </c>
       <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AA11" si="7">IF(OR(Y3=FALSE,Z3=FALSE),"None","")</f>
+        <f t="shared" ref="AA3:AA11" si="6">IF(OR(Y3=FALSE,Z3=FALSE),"None","")</f>
         <v>None</v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB11" si="8">IF(OR(Y3=FALSE,Z3=FALSE),"None","")</f>
+        <f t="shared" ref="AB3:AB11" si="7">IF(OR(Y3=FALSE,Z3=FALSE),"None","")</f>
         <v>None</v>
       </c>
       <c r="AC3" t="b">
@@ -4870,7 +4865,7 @@
         <v>1</v>
       </c>
       <c r="AI3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3" t="b">
         <v>0</v>
@@ -4885,21 +4880,21 @@
         <v>0</v>
       </c>
       <c r="AN3" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>101</v>
+      <c r="A4" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>82</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -4910,78 +4905,77 @@
         <v>None</v>
       </c>
       <c r="G4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="str">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="str">
         <f t="shared" si="2"/>
         <v>None</v>
       </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" t="str">
+      <c r="M4" t="str">
         <f t="shared" si="3"/>
         <v>None</v>
       </c>
-      <c r="M4" t="str">
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" t="str">
         <f t="shared" si="4"/>
         <v>None</v>
       </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4" t="b">
-        <v>0</v>
-      </c>
-      <c r="T4" t="str">
+      <c r="U4" t="str">
         <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="U4" t="str">
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+      <c r="W4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="str">
         <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="V4" t="b">
-        <v>0</v>
-      </c>
-      <c r="W4" t="b">
-        <v>1</v>
-      </c>
-      <c r="X4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="str">
+      <c r="AB4" t="str">
         <f t="shared" si="7"/>
         <v>None</v>
       </c>
-      <c r="AB4" t="str">
-        <f t="shared" si="8"/>
-        <v>None</v>
-      </c>
       <c r="AC4" t="b">
         <v>0</v>
       </c>
@@ -5001,7 +4995,7 @@
         <v>1</v>
       </c>
       <c r="AI4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4" t="b">
         <v>0</v>
@@ -5016,15 +5010,15 @@
         <v>0</v>
       </c>
       <c r="AN4" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>102</v>
+      <c r="A5" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -5068,7 +5062,7 @@
         <v>1</v>
       </c>
       <c r="P5" t="str">
-        <f t="shared" ref="P5:P10" si="9">IF(AND(O5=TRUE,G5=TRUE),"","None")</f>
+        <f t="shared" ref="P5:P10" si="8">IF(AND(O5=TRUE,G5=TRUE),"","None")</f>
         <v>None</v>
       </c>
       <c r="Q5" t="b">
@@ -5081,36 +5075,36 @@
         <v>0</v>
       </c>
       <c r="T5" t="str">
+        <f t="shared" si="4"/>
+        <v>None</v>
+      </c>
+      <c r="U5" t="str">
         <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="U5" t="str">
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W5" t="b">
+        <v>1</v>
+      </c>
+      <c r="X5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="str">
         <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="V5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W5" t="b">
-        <v>1</v>
-      </c>
-      <c r="X5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="str">
+      <c r="AB5" t="str">
         <f t="shared" si="7"/>
         <v>None</v>
       </c>
-      <c r="AB5" t="str">
-        <f t="shared" si="8"/>
-        <v>None</v>
-      </c>
       <c r="AC5" t="b">
         <v>0</v>
       </c>
@@ -5146,8 +5140,8 @@
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>103</v>
+      <c r="A6" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
@@ -5156,87 +5150,86 @@
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>80</v>
       </c>
       <c r="G6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="str">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="str">
         <f t="shared" si="2"/>
         <v>None</v>
       </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" t="str">
+      <c r="M6" t="str">
         <f t="shared" si="3"/>
         <v>None</v>
       </c>
-      <c r="M6" t="str">
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" t="str">
         <f t="shared" si="4"/>
         <v>None</v>
       </c>
-      <c r="N6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" t="str">
+      <c r="U6" t="str">
         <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="U6" t="str">
+      <c r="V6" t="b">
+        <v>0</v>
+      </c>
+      <c r="W6" t="b">
+        <v>1</v>
+      </c>
+      <c r="X6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="str">
         <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="V6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W6" t="b">
-        <v>1</v>
-      </c>
-      <c r="X6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="str">
+      <c r="AB6" t="str">
         <f t="shared" si="7"/>
         <v>None</v>
       </c>
-      <c r="AB6" t="str">
-        <f t="shared" si="8"/>
-        <v>None</v>
-      </c>
       <c r="AC6" t="b">
         <v>0</v>
       </c>
@@ -5256,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="AI6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6" t="b">
         <v>0</v>
@@ -5271,15 +5264,15 @@
         <v>0</v>
       </c>
       <c r="AN6" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>104</v>
+      <c r="A7" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -5311,63 +5304,63 @@
         <v>0</v>
       </c>
       <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>None</v>
+      </c>
+      <c r="M7" t="str">
         <f t="shared" si="3"/>
         <v>None</v>
       </c>
-      <c r="M7" t="str">
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="8"/>
+        <v>None</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" t="str">
         <f t="shared" si="4"/>
         <v>None</v>
       </c>
-      <c r="N7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" t="b">
-        <v>1</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" si="9"/>
-        <v>None</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>0</v>
-      </c>
-      <c r="R7" t="b">
-        <v>1</v>
-      </c>
-      <c r="S7" t="b">
-        <v>0</v>
-      </c>
-      <c r="T7" t="str">
+      <c r="U7" t="str">
         <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="U7" t="str">
+      <c r="V7" t="b">
+        <v>0</v>
+      </c>
+      <c r="W7" t="b">
+        <v>1</v>
+      </c>
+      <c r="X7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="str">
         <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="V7" t="b">
-        <v>0</v>
-      </c>
-      <c r="W7" t="b">
-        <v>1</v>
-      </c>
-      <c r="X7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA7" t="str">
+      <c r="AB7" t="str">
         <f t="shared" si="7"/>
         <v>None</v>
       </c>
-      <c r="AB7" t="str">
-        <f t="shared" si="8"/>
-        <v>None</v>
-      </c>
       <c r="AC7" t="b">
         <v>0</v>
       </c>
@@ -5403,17 +5396,17 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>105</v>
+      <c r="A8" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="B8" t="s">
         <v>82</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -5424,78 +5417,77 @@
         <v>None</v>
       </c>
       <c r="G8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="str">
+        <v>1</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" t="str">
         <f t="shared" si="2"/>
         <v>None</v>
       </c>
-      <c r="J8" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <f t="shared" si="3"/>
         <v>None</v>
       </c>
-      <c r="M8" t="str">
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8" t="str">
         <f t="shared" si="4"/>
         <v>None</v>
       </c>
-      <c r="N8" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" t="b">
-        <v>1</v>
-      </c>
-      <c r="P8" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="b">
-        <v>1</v>
-      </c>
-      <c r="R8" t="b">
-        <v>1</v>
-      </c>
-      <c r="S8" t="b">
-        <v>0</v>
-      </c>
-      <c r="T8" t="str">
+      <c r="U8" t="str">
         <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="U8" t="str">
+      <c r="V8" t="b">
+        <v>0</v>
+      </c>
+      <c r="W8" t="b">
+        <v>1</v>
+      </c>
+      <c r="X8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="str">
         <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="V8" t="b">
-        <v>0</v>
-      </c>
-      <c r="W8" t="b">
-        <v>1</v>
-      </c>
-      <c r="X8" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y8" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA8" t="str">
+      <c r="AB8" t="str">
         <f t="shared" si="7"/>
         <v>None</v>
       </c>
-      <c r="AB8" t="str">
-        <f t="shared" si="8"/>
-        <v>None</v>
-      </c>
       <c r="AC8" t="b">
         <v>0</v>
       </c>
@@ -5503,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="AE8" t="str">
-        <f t="shared" ref="AE8" si="10">IF(AD8=FALSE,"","None")</f>
+        <f t="shared" ref="AE8" si="9">IF(AD8=FALSE,"","None")</f>
         <v>None</v>
       </c>
       <c r="AF8" t="b">
@@ -5531,12 +5523,12 @@
         <v>0</v>
       </c>
       <c r="AN8" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>99</v>
+      <c r="A9" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="B9" t="s">
         <v>75</v>
@@ -5569,63 +5561,63 @@
         <v>0</v>
       </c>
       <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>None</v>
+      </c>
+      <c r="M9" t="str">
         <f t="shared" si="3"/>
         <v>None</v>
       </c>
-      <c r="M9" t="str">
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="8"/>
+        <v>None</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" t="str">
         <f t="shared" si="4"/>
         <v>None</v>
       </c>
-      <c r="N9" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" t="b">
-        <v>1</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" si="9"/>
-        <v>None</v>
-      </c>
-      <c r="Q9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R9" t="b">
-        <v>1</v>
-      </c>
-      <c r="S9" t="b">
-        <v>0</v>
-      </c>
-      <c r="T9" t="str">
+      <c r="U9" t="str">
         <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="U9" t="str">
+      <c r="V9" t="b">
+        <v>0</v>
+      </c>
+      <c r="W9" t="b">
+        <v>1</v>
+      </c>
+      <c r="X9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="str">
         <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="V9" t="b">
-        <v>0</v>
-      </c>
-      <c r="W9" t="b">
-        <v>1</v>
-      </c>
-      <c r="X9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA9" t="str">
+      <c r="AB9" t="str">
         <f t="shared" si="7"/>
         <v>None</v>
       </c>
-      <c r="AB9" t="str">
-        <f t="shared" si="8"/>
-        <v>None</v>
-      </c>
       <c r="AC9" t="b">
         <v>0</v>
       </c>
@@ -5661,8 +5653,8 @@
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>106</v>
+      <c r="A10" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B10" t="s">
         <v>75</v>
@@ -5697,63 +5689,63 @@
         <v>0</v>
       </c>
       <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>None</v>
+      </c>
+      <c r="M10" t="str">
         <f t="shared" si="3"/>
         <v>None</v>
       </c>
-      <c r="M10" t="str">
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="8"/>
+        <v>None</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+      <c r="S10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T10" t="str">
         <f t="shared" si="4"/>
         <v>None</v>
       </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" t="b">
-        <v>1</v>
-      </c>
-      <c r="P10" t="str">
-        <f t="shared" si="9"/>
-        <v>None</v>
-      </c>
-      <c r="Q10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R10" t="b">
-        <v>1</v>
-      </c>
-      <c r="S10" t="b">
-        <v>0</v>
-      </c>
-      <c r="T10" t="str">
+      <c r="U10" t="str">
         <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="U10" t="str">
+      <c r="V10" t="b">
+        <v>0</v>
+      </c>
+      <c r="W10" t="b">
+        <v>1</v>
+      </c>
+      <c r="X10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="str">
         <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="V10" t="b">
-        <v>0</v>
-      </c>
-      <c r="W10" t="b">
-        <v>1</v>
-      </c>
-      <c r="X10" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y10" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA10" t="str">
+      <c r="AB10" t="str">
         <f t="shared" si="7"/>
         <v>None</v>
       </c>
-      <c r="AB10" t="str">
-        <f t="shared" si="8"/>
-        <v>None</v>
-      </c>
       <c r="AC10" t="b">
         <v>0</v>
       </c>
@@ -5789,8 +5781,8 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>107</v>
+      <c r="A11" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="B11" t="s">
         <v>82</v>
@@ -5816,7 +5808,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I3:I11" si="10">IF(H11=TRUE,"","None")</f>
         <v>None</v>
       </c>
       <c r="J11" t="b">
@@ -5871,11 +5863,11 @@
         <v>0</v>
       </c>
       <c r="AA11" t="str">
+        <f t="shared" si="6"/>
+        <v>None</v>
+      </c>
+      <c r="AB11" t="str">
         <f t="shared" si="7"/>
-        <v>None</v>
-      </c>
-      <c r="AB11" t="str">
-        <f t="shared" si="8"/>
         <v>None</v>
       </c>
       <c r="AC11" t="b">
@@ -5924,7 +5916,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6009,10 +6001,10 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -6091,17 +6083,17 @@
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>124</v>
+      <c r="A2" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="B2" t="s">
         <v>82</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="str">
         <f>IF(OR(C2=FALSE,D2=FALSE),"None","")</f>
@@ -6112,14 +6104,13 @@
         <v>None</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="str">
-        <f>IF(H2=TRUE,"","None")</f>
-        <v>None</v>
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -6141,8 +6132,8 @@
       <c r="O2" t="b">
         <v>1</v>
       </c>
-      <c r="P2" t="b">
-        <v>0</v>
+      <c r="P2" t="s">
+        <v>80</v>
       </c>
       <c r="Q2" t="b">
         <v>1</v>
@@ -6202,7 +6193,7 @@
         <v>None</v>
       </c>
       <c r="AI2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2" t="b">
         <v>0</v>
@@ -6217,12 +6208,12 @@
         <v>0</v>
       </c>
       <c r="AN2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>112</v>
+      <c r="A3" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="B3" t="s">
         <v>75</v>
@@ -6350,8 +6341,8 @@
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>126</v>
+      <c r="A4" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="B4" t="s">
         <v>77</v>
@@ -6474,12 +6465,12 @@
         <v>0</v>
       </c>
       <c r="AN4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>109</v>
+      <c r="A5" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
@@ -6605,11 +6596,11 @@
         <v>0</v>
       </c>
       <c r="AN5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B6" t="s">
@@ -6734,12 +6725,12 @@
         <v>0</v>
       </c>
       <c r="AN6" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>127</v>
+      <c r="A7" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
@@ -6867,7 +6858,7 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
@@ -6993,10 +6984,10 @@
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -7120,7 +7111,7 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
         <v>75</v>
@@ -7245,7 +7236,7 @@
         <v>0</v>
       </c>
       <c r="AN10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -7258,9 +7249,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A598A86-A726-4035-A5D8-7FB05BCB0D54}">
   <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="AL1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK12" sqref="AK12"/>
+      <selection pane="bottomLeft" activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7345,10 +7336,10 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -7428,10 +7419,10 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -7556,7 +7547,7 @@
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
@@ -7684,7 +7675,7 @@
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>77</v>
@@ -7693,23 +7684,22 @@
         <v>1</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>80</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
+      <c r="F4" t="s">
+        <v>80</v>
       </c>
       <c r="G4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" ref="I4" si="9">IF(H4=TRUE,"","None")</f>
-        <v>None</v>
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -7731,8 +7721,8 @@
       <c r="O4" t="b">
         <v>1</v>
       </c>
-      <c r="P4" t="b">
-        <v>0</v>
+      <c r="P4" t="s">
+        <v>80</v>
       </c>
       <c r="Q4" t="b">
         <v>1</v>
@@ -7793,7 +7783,7 @@
         <v>0</v>
       </c>
       <c r="AI4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4" t="b">
         <v>0</v>
@@ -7806,14 +7796,17 @@
       </c>
       <c r="AM4" t="b">
         <v>0</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -7938,7 +7931,7 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
         <v>75</v>
@@ -8066,10 +8059,10 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -8194,7 +8187,7 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
@@ -8316,12 +8309,12 @@
         <v>0</v>
       </c>
       <c r="AN8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
         <v>82</v>
@@ -8449,10 +8442,10 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -8577,7 +8570,7 @@
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
@@ -8713,9 +8706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE99220F-96BB-4653-9C1B-82FB7B184800}">
   <dimension ref="A1:AO6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1048548" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1048576" sqref="A1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8800,10 +8793,10 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -8883,7 +8876,7 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
@@ -9006,10 +8999,10 @@
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -9133,10 +9126,10 @@
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -9258,10 +9251,10 @@
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -9385,7 +9378,7 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
@@ -9394,22 +9387,22 @@
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>80</v>
       </c>
-      <c r="F6" t="b">
-        <v>1</v>
+      <c r="F6" t="s">
+        <v>80</v>
       </c>
       <c r="G6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -9431,8 +9424,8 @@
       <c r="O6" t="b">
         <v>1</v>
       </c>
-      <c r="P6" t="b">
-        <v>0</v>
+      <c r="P6" t="s">
+        <v>80</v>
       </c>
       <c r="Q6" t="b">
         <v>1</v>
@@ -9493,7 +9486,7 @@
         <v>None</v>
       </c>
       <c r="AI6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6" t="b">
         <v>0</v>
@@ -9506,6 +9499,9 @@
       </c>
       <c r="AM6" t="b">
         <v>0</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -9565,7 +9561,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -9573,7 +9569,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9642,18 +9638,18 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>